<commit_message>
fixes access to indexes
</commit_message>
<xml_diff>
--- a/indexes.xlsx
+++ b/indexes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="decomposition" sheetId="4" r:id="rId1"/>
@@ -1879,9 +1879,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AMK48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2803,8 +2801,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G455"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>